<commit_message>
Changed spreadsheet data to match output.txt
</commit_message>
<xml_diff>
--- a/lab03-results.xlsx
+++ b/lab03-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\DC2310\T3\collections_ADTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C02D427-0B6F-4A13-8057-EE7554345702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C4A1B-446D-41C7-A75B-135CC1CBD4ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,12 +72,6 @@
     <t>75K</t>
   </si>
   <si>
-    <t>Pick 100 Words</t>
-  </si>
-  <si>
-    <t>Remove 100 Words</t>
-  </si>
-  <si>
     <t>Array</t>
   </si>
   <si>
@@ -121,6 +115,12 @@
   </si>
   <si>
     <t>O(n log n)</t>
+  </si>
+  <si>
+    <t>Pick 1000 Words</t>
+  </si>
+  <si>
+    <t>Remove 1000 Words</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1245,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Pick 100 words</a:t>
+              <a:t>Pick 1000 words</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1281,7 +1281,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1163778673036866"/>
+          <c:y val="0.17071049575517133"/>
+          <c:w val="0.72676008847772078"/>
+          <c:h val="0.61452582838779934"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1338,16 +1348,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,7 +1414,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1413,7 +1423,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1478,16 +1488,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,16 +1562,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,16 +1636,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1700,16 +1710,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81</c:v>
+                  <c:v>348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1722,7 +1732,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1844,7 +1853,6 @@
         <c:axId val="1314473456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2075,7 +2083,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Remove 100 words</a:t>
+              <a:t>Remove 1000 words</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2168,16 +2176,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2242,16 +2250,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2316,16 +2324,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2390,16 +2398,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2464,16 +2472,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,16 +2546,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2560,7 +2568,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4588,11 +4595,11 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>144769</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>172586</xdr:rowOff>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>293687</xdr:colOff>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4957,8 +4964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5007,7 +5014,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
@@ -5114,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -5137,28 +5144,28 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="6">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13" s="6">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="F13" s="6">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="G13" s="6">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="H13" s="6">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5169,22 +5176,22 @@
         <v>10</v>
       </c>
       <c r="C14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F14" s="6">
-        <v>20</v>
+        <v>194</v>
       </c>
       <c r="G14" s="6">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="H14" s="6">
-        <v>28</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5195,22 +5202,22 @@
         <v>12</v>
       </c>
       <c r="C15" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="F15" s="6">
-        <v>50</v>
+        <v>510</v>
       </c>
       <c r="G15" s="6">
-        <v>24</v>
+        <v>161</v>
       </c>
       <c r="H15" s="6">
-        <v>55</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5221,22 +5228,22 @@
         <v>14</v>
       </c>
       <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
       <c r="E16" s="6">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="F16" s="6">
-        <v>73</v>
+        <v>630</v>
       </c>
       <c r="G16" s="6">
-        <v>86</v>
+        <v>203</v>
       </c>
       <c r="H16" s="6">
-        <v>81</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5244,7 +5251,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>2</v>
@@ -5267,28 +5274,28 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D22" s="6">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E22" s="6">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F22" s="6">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="G22" s="6">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="H22" s="6">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5299,22 +5306,22 @@
         <v>10</v>
       </c>
       <c r="C23" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="6">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="F23" s="6">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="G23" s="6">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="H23" s="6">
-        <v>24</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5325,22 +5332,22 @@
         <v>12</v>
       </c>
       <c r="C24" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="F24" s="6">
-        <v>43</v>
+        <v>463</v>
       </c>
       <c r="G24" s="6">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="H24" s="6">
-        <v>55</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5351,22 +5358,22 @@
         <v>14</v>
       </c>
       <c r="C25" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D25" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E25" s="6">
-        <v>16</v>
+        <v>139</v>
       </c>
       <c r="F25" s="6">
-        <v>65</v>
+        <v>612</v>
       </c>
       <c r="G25" s="6">
-        <v>79</v>
+        <v>193</v>
       </c>
       <c r="H25" s="6">
-        <v>53</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
@@ -5381,45 +5388,45 @@
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="I45" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q45" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
@@ -5427,7 +5434,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="10"/>
@@ -5436,13 +5443,13 @@
         <v>2</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>2</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
@@ -5450,7 +5457,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="10"/>
@@ -5459,13 +5466,13 @@
         <v>3</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q47" s="6" t="s">
         <v>3</v>
       </c>
       <c r="R47" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
@@ -5473,7 +5480,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="10"/>
@@ -5482,13 +5489,13 @@
         <v>4</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q48" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
@@ -5496,7 +5503,7 @@
         <v>5</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="10"/>
@@ -5505,13 +5512,13 @@
         <v>5</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q49" s="6" t="s">
         <v>5</v>
       </c>
       <c r="R49" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
@@ -5519,7 +5526,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="10"/>
@@ -5528,13 +5535,13 @@
         <v>6</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q50" s="6" t="s">
         <v>6</v>
       </c>
       <c r="R50" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
@@ -5542,7 +5549,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="10"/>
@@ -5551,13 +5558,13 @@
         <v>7</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q51" s="6" t="s">
         <v>7</v>
       </c>
       <c r="R51" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
@@ -5576,7 +5583,7 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>